<commit_message>
jump animations are in updates to gameboard/playstate to support death animations better/properly/whatever
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="162">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>don't allow map rotation when processing at all</t>
+  </si>
+  <si>
+    <t>death animation isn't drawing now for some reason</t>
   </si>
 </sst>
 </file>
@@ -938,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K218"/>
+  <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1726,34 +1729,43 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="10" customFormat="1">
-      <c r="D84" s="10" t="s">
-        <v>157</v>
+    <row r="84" spans="1:4" s="6" customFormat="1">
+      <c r="A84" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" s="7">
+        <v>39962</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="10" customFormat="1">
       <c r="D85" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="10" customFormat="1">
+      <c r="D86" s="10" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="2" customFormat="1">
-      <c r="D86" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="2" customFormat="1">
       <c r="D87" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="2" customFormat="1">
       <c r="D88" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="2" customFormat="1">
       <c r="D89" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="2" customFormat="1">
@@ -1761,25 +1773,16 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="2" customFormat="1"/>
-    <row r="92" spans="1:4" s="3" customFormat="1"/>
-    <row r="93" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D93" s="5" t="s">
+    <row r="91" spans="1:4" s="2" customFormat="1">
+      <c r="D91" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="2" customFormat="1"/>
+    <row r="93" spans="1:4" s="3" customFormat="1"/>
+    <row r="94" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D94" s="5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" s="6" customFormat="1">
-      <c r="A94" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C94" s="7">
-        <v>39954</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="6" customFormat="1">
@@ -1793,7 +1796,7 @@
         <v>39954</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="6" customFormat="1">
@@ -1807,7 +1810,7 @@
         <v>39954</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="6" customFormat="1">
@@ -1815,13 +1818,13 @@
         <v>80</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C97" s="7">
-        <v>39955</v>
+        <v>39954</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="6" customFormat="1">
@@ -1835,7 +1838,7 @@
         <v>39955</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="6" customFormat="1">
@@ -1849,7 +1852,7 @@
         <v>39955</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="6" customFormat="1">
@@ -1863,7 +1866,7 @@
         <v>39955</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="6" customFormat="1">
@@ -1871,13 +1874,13 @@
         <v>80</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C101" s="7">
         <v>39955</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="6" customFormat="1">
@@ -1885,27 +1888,27 @@
         <v>80</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C102" s="7">
         <v>39955</v>
       </c>
       <c r="D102" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="6" customFormat="1">
+      <c r="A103" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" s="7">
+        <v>39955</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" s="14" customFormat="1">
-      <c r="A103" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C103" s="15">
-        <v>39955</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="14" customFormat="1">
@@ -1916,24 +1919,24 @@
         <v>79</v>
       </c>
       <c r="C104" s="15">
+        <v>39955</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="14" customFormat="1">
+      <c r="A105" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C105" s="15">
         <v>39956</v>
       </c>
-      <c r="D104" s="14" t="s">
+      <c r="D105" s="14" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" s="6" customFormat="1">
-      <c r="A105" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C105" s="7">
-        <v>39957</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="6" customFormat="1">
@@ -1947,7 +1950,7 @@
         <v>39957</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="6" customFormat="1">
@@ -1961,7 +1964,7 @@
         <v>39957</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="6" customFormat="1">
@@ -1975,7 +1978,7 @@
         <v>39957</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="6" customFormat="1">
@@ -1983,13 +1986,13 @@
         <v>80</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>136</v>
+        <v>79</v>
       </c>
       <c r="C109" s="7">
-        <v>39959</v>
+        <v>39957</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="6" customFormat="1">
@@ -2003,7 +2006,7 @@
         <v>39959</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="6" customFormat="1">
@@ -2017,7 +2020,7 @@
         <v>39959</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="6" customFormat="1">
@@ -2031,7 +2034,7 @@
         <v>39959</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="6" customFormat="1">
@@ -2045,56 +2048,56 @@
         <v>39959</v>
       </c>
       <c r="D113" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" s="6" customFormat="1">
+      <c r="A114" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C114" s="7">
+        <v>39959</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="114" spans="1:4" s="2" customFormat="1">
-      <c r="D114" s="2" t="s">
+    <row r="115" spans="1:4" s="2" customFormat="1">
+      <c r="D115" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:4" s="2" customFormat="1">
-      <c r="C115" s="16"/>
-      <c r="D115" s="2" t="s">
+    <row r="116" spans="1:4" s="2" customFormat="1">
+      <c r="C116" s="16"/>
+      <c r="D116" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" s="2" customFormat="1">
-      <c r="D116" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="2" customFormat="1">
       <c r="D117" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="2" customFormat="1">
       <c r="D118" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" s="2" customFormat="1">
+      <c r="D119" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="119" spans="1:4" s="2" customFormat="1"/>
     <row r="120" spans="1:4" s="2" customFormat="1"/>
-    <row r="121" spans="1:4" s="3" customFormat="1"/>
+    <row r="121" spans="1:4" s="2" customFormat="1"/>
     <row r="122" spans="1:4" s="3" customFormat="1"/>
-    <row r="123" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D123" s="5" t="s">
+    <row r="123" spans="1:4" s="3" customFormat="1"/>
+    <row r="124" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D124" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" s="6" customFormat="1">
-      <c r="A124" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C124" s="7">
-        <v>39953</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="6" customFormat="1">
@@ -2108,7 +2111,7 @@
         <v>39953</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="6" customFormat="1">
@@ -2122,7 +2125,7 @@
         <v>39953</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="6" customFormat="1">
@@ -2136,21 +2139,21 @@
         <v>39953</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" s="7" customFormat="1">
-      <c r="A128" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B128" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" s="6" customFormat="1">
+      <c r="A128" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C128" s="7">
         <v>39953</v>
       </c>
-      <c r="D128" s="7" t="s">
-        <v>71</v>
+      <c r="D128" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="7" customFormat="1">
@@ -2161,60 +2164,60 @@
         <v>94</v>
       </c>
       <c r="C129" s="7">
+        <v>39953</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="7" customFormat="1">
+      <c r="A130" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C130" s="7">
         <v>39954</v>
       </c>
-      <c r="D129" s="7" t="s">
+      <c r="D130" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="7" customFormat="1">
-      <c r="D130" s="7" t="s">
+    <row r="131" spans="1:5" s="7" customFormat="1">
+      <c r="D131" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="3" customFormat="1"/>
     <row r="132" spans="1:5" s="3" customFormat="1"/>
-    <row r="133" spans="1:5" s="4" customFormat="1" ht="26.25">
-      <c r="D133" s="5" t="s">
+    <row r="133" spans="1:5" s="3" customFormat="1"/>
+    <row r="134" spans="1:5" s="4" customFormat="1" ht="26.25">
+      <c r="D134" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="2" customFormat="1">
-      <c r="D134" s="2" t="s">
+    <row r="135" spans="1:5" s="2" customFormat="1">
+      <c r="D135" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="3" customFormat="1"/>
     <row r="136" spans="1:5" s="3" customFormat="1"/>
-    <row r="137" spans="1:5" s="4" customFormat="1" ht="26.25">
-      <c r="D137" s="5" t="s">
+    <row r="137" spans="1:5" s="3" customFormat="1"/>
+    <row r="138" spans="1:5" s="4" customFormat="1" ht="26.25">
+      <c r="D138" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="12" customFormat="1">
-      <c r="D138" s="12" t="s">
+    <row r="139" spans="1:5" s="12" customFormat="1">
+      <c r="D139" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="3" customFormat="1"/>
     <row r="140" spans="1:5" s="3" customFormat="1"/>
-    <row r="141" spans="1:5" s="4" customFormat="1" ht="26.25">
-      <c r="D141" s="5" t="s">
+    <row r="141" spans="1:5" s="3" customFormat="1"/>
+    <row r="142" spans="1:5" s="4" customFormat="1" ht="26.25">
+      <c r="D142" s="5" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" s="6" customFormat="1">
-      <c r="A142" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B142" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C142" s="7">
-        <v>39955</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="143" spans="1:5" s="6" customFormat="1">
@@ -2227,8 +2230,8 @@
       <c r="C143" s="7">
         <v>39955</v>
       </c>
-      <c r="E143" s="6" t="s">
-        <v>92</v>
+      <c r="D143" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="6" customFormat="1">
@@ -2241,28 +2244,28 @@
       <c r="C144" s="7">
         <v>39955</v>
       </c>
-      <c r="D144" s="6" t="s">
+      <c r="E144" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" s="6" customFormat="1">
+      <c r="A145" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C145" s="7">
+        <v>39955</v>
+      </c>
+      <c r="D145" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="1:4" s="3" customFormat="1"/>
-    <row r="146" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D146" s="5" t="s">
+    <row r="146" spans="1:4" s="3" customFormat="1"/>
+    <row r="147" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D147" s="5" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" s="6" customFormat="1">
-      <c r="A147" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C147" s="7">
-        <v>39955</v>
-      </c>
-      <c r="D147" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:4" s="6" customFormat="1">
@@ -2276,7 +2279,7 @@
         <v>39955</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:4" s="6" customFormat="1">
@@ -2290,7 +2293,7 @@
         <v>39955</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="150" spans="1:4" s="6" customFormat="1">
@@ -2298,13 +2301,13 @@
         <v>80</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C150" s="7">
         <v>39955</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="151" spans="1:4" s="6" customFormat="1">
@@ -2312,13 +2315,13 @@
         <v>80</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C151" s="7">
         <v>39955</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="152" spans="1:4" s="6" customFormat="1">
@@ -2326,87 +2329,87 @@
         <v>80</v>
       </c>
       <c r="B152" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C152" s="7">
+        <v>39955</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" s="6" customFormat="1">
+      <c r="A153" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B153" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C152" s="7">
+      <c r="C153" s="7">
         <v>39957</v>
       </c>
-      <c r="D152" s="6" t="s">
+      <c r="D153" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="153" spans="1:4" s="3" customFormat="1"/>
-    <row r="154" spans="1:4" s="9" customFormat="1" ht="28.5">
-      <c r="D154" s="9" t="s">
+    <row r="154" spans="1:4" s="3" customFormat="1"/>
+    <row r="155" spans="1:4" s="9" customFormat="1" ht="28.5">
+      <c r="D155" s="9" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" s="12" customFormat="1">
-      <c r="D155" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="156" spans="1:4" s="12" customFormat="1">
       <c r="D156" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="157" spans="1:4" s="12" customFormat="1">
       <c r="D157" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" s="12" customFormat="1">
+      <c r="D158" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="158" spans="1:4" s="3" customFormat="1"/>
-    <row r="159" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D159" s="5" t="s">
+    <row r="159" spans="1:4" s="3" customFormat="1"/>
+    <row r="160" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D160" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="160" spans="1:4" s="6" customFormat="1">
-      <c r="A160" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C160" s="7">
+    <row r="161" spans="1:4" s="6" customFormat="1">
+      <c r="A161" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C161" s="7">
         <v>39957</v>
       </c>
-      <c r="D160" s="6" t="s">
+      <c r="D161" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="161" spans="1:4" s="2" customFormat="1"/>
-    <row r="162" spans="1:4" s="3" customFormat="1"/>
-    <row r="163" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D163" s="5" t="s">
+    <row r="162" spans="1:4" s="2" customFormat="1"/>
+    <row r="163" spans="1:4" s="3" customFormat="1"/>
+    <row r="164" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D164" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:4" s="2" customFormat="1">
-      <c r="D164" s="2" t="s">
+    <row r="165" spans="1:4" s="2" customFormat="1">
+      <c r="D165" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="165" spans="1:4" s="3" customFormat="1"/>
     <row r="166" spans="1:4" s="3" customFormat="1"/>
-    <row r="167" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D167" s="5" t="s">
+    <row r="167" spans="1:4" s="3" customFormat="1"/>
+    <row r="168" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D168" s="5" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" s="6" customFormat="1">
-      <c r="A168" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C168" s="7">
-        <v>39957</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="169" spans="1:4" s="6" customFormat="1">
@@ -2420,7 +2423,7 @@
         <v>39957</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="6" customFormat="1">
@@ -2434,7 +2437,7 @@
         <v>39957</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="171" spans="1:4" s="6" customFormat="1">
@@ -2448,22 +2451,35 @@
         <v>39957</v>
       </c>
       <c r="D171" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" s="6" customFormat="1">
+      <c r="A172" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C172" s="7">
+        <v>39957</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="172" spans="1:4" s="2" customFormat="1"/>
     <row r="173" spans="1:4" s="2" customFormat="1"/>
-    <row r="174" spans="1:4" s="2" customFormat="1">
-      <c r="D174" s="2" t="s">
+    <row r="174" spans="1:4" s="2" customFormat="1"/>
+    <row r="175" spans="1:4" s="2" customFormat="1">
+      <c r="D175" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="175" spans="1:4" s="2" customFormat="1"/>
     <row r="176" spans="1:4" s="2" customFormat="1"/>
     <row r="177" s="2" customFormat="1"/>
     <row r="178" s="2" customFormat="1"/>
     <row r="179" s="2" customFormat="1"/>
-    <row r="180" s="3" customFormat="1"/>
+    <row r="180" s="2" customFormat="1"/>
     <row r="181" s="3" customFormat="1"/>
     <row r="182" s="3" customFormat="1"/>
     <row r="183" s="3" customFormat="1"/>
@@ -2502,6 +2518,7 @@
     <row r="216" s="3" customFormat="1"/>
     <row r="217" s="3" customFormat="1"/>
     <row r="218" s="3" customFormat="1"/>
+    <row r="219" s="3" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
electric animation death fixed
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="170">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>electric death animation isn't drawing now for some reason</t>
+  </si>
+  <si>
+    <t>level select state images are glitching out</t>
   </si>
 </sst>
 </file>
@@ -969,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K225"/>
+  <dimension ref="A1:K226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1898,8 +1901,17 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="2" customFormat="1">
-      <c r="D93" s="2" t="s">
+    <row r="93" spans="1:4" s="6" customFormat="1">
+      <c r="A93" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C93" s="7">
+        <v>39964</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2555,78 +2567,78 @@
         <v>106</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="3" customFormat="1"/>
-    <row r="161" spans="1:4" s="9" customFormat="1" ht="28.5">
-      <c r="D161" s="9" t="s">
+    <row r="160" spans="1:5" s="6" customFormat="1">
+      <c r="A160" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C160" s="7">
+        <v>39964</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" s="3" customFormat="1"/>
+    <row r="162" spans="1:4" s="9" customFormat="1" ht="28.5">
+      <c r="D162" s="9" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" s="12" customFormat="1">
-      <c r="D162" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="163" spans="1:4" s="12" customFormat="1">
       <c r="D163" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="164" spans="1:4" s="12" customFormat="1">
       <c r="D164" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" s="12" customFormat="1">
+      <c r="D165" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="165" spans="1:4" s="3" customFormat="1"/>
-    <row r="166" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D166" s="5" t="s">
+    <row r="166" spans="1:4" s="3" customFormat="1"/>
+    <row r="167" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D167" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="6" customFormat="1">
-      <c r="A167" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C167" s="7">
+    <row r="168" spans="1:4" s="6" customFormat="1">
+      <c r="A168" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C168" s="7">
         <v>39957</v>
       </c>
-      <c r="D167" s="6" t="s">
+      <c r="D168" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="168" spans="1:4" s="2" customFormat="1"/>
-    <row r="169" spans="1:4" s="3" customFormat="1"/>
-    <row r="170" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D170" s="5" t="s">
+    <row r="169" spans="1:4" s="2" customFormat="1"/>
+    <row r="170" spans="1:4" s="3" customFormat="1"/>
+    <row r="171" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D171" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:4" s="2" customFormat="1">
-      <c r="D171" s="2" t="s">
+    <row r="172" spans="1:4" s="2" customFormat="1">
+      <c r="D172" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="172" spans="1:4" s="3" customFormat="1"/>
     <row r="173" spans="1:4" s="3" customFormat="1"/>
-    <row r="174" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D174" s="5" t="s">
+    <row r="174" spans="1:4" s="3" customFormat="1"/>
+    <row r="175" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D175" s="5" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" s="6" customFormat="1">
-      <c r="A175" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B175" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C175" s="7">
-        <v>39957</v>
-      </c>
-      <c r="D175" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="176" spans="1:4" s="6" customFormat="1">
@@ -2640,7 +2652,7 @@
         <v>39957</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="177" spans="1:4" s="6" customFormat="1">
@@ -2654,7 +2666,7 @@
         <v>39957</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="178" spans="1:4" s="6" customFormat="1">
@@ -2668,22 +2680,35 @@
         <v>39957</v>
       </c>
       <c r="D178" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" s="6" customFormat="1">
+      <c r="A179" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C179" s="7">
+        <v>39957</v>
+      </c>
+      <c r="D179" s="6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="179" spans="1:4" s="2" customFormat="1"/>
     <row r="180" spans="1:4" s="2" customFormat="1"/>
-    <row r="181" spans="1:4" s="2" customFormat="1">
-      <c r="D181" s="2" t="s">
+    <row r="181" spans="1:4" s="2" customFormat="1"/>
+    <row r="182" spans="1:4" s="2" customFormat="1">
+      <c r="D182" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="182" spans="1:4" s="2" customFormat="1"/>
     <row r="183" spans="1:4" s="2" customFormat="1"/>
     <row r="184" spans="1:4" s="2" customFormat="1"/>
     <row r="185" spans="1:4" s="2" customFormat="1"/>
     <row r="186" spans="1:4" s="2" customFormat="1"/>
-    <row r="187" spans="1:4" s="3" customFormat="1"/>
+    <row r="187" spans="1:4" s="2" customFormat="1"/>
     <row r="188" spans="1:4" s="3" customFormat="1"/>
     <row r="189" spans="1:4" s="3" customFormat="1"/>
     <row r="190" spans="1:4" s="3" customFormat="1"/>
@@ -2722,6 +2747,7 @@
     <row r="223" s="3" customFormat="1"/>
     <row r="224" s="3" customFormat="1"/>
     <row r="225" s="3" customFormat="1"/>
+    <row r="226" s="3" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
jump animation code is done any "bugs" you find are features
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="157">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>robot dies not come back to life after dying to electricity</t>
+  </si>
+  <si>
+    <t>robot draw order  during jumps needs to be adjusted</t>
+  </si>
+  <si>
+    <t>Dave/Tom</t>
   </si>
 </sst>
 </file>
@@ -912,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2474,182 +2480,199 @@
       </c>
     </row>
     <row r="112" spans="1:4" s="6" customFormat="1">
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
+      <c r="A112" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C112" s="7">
+        <v>39964</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="113" spans="2:4" s="6" customFormat="1">
-      <c r="B113" s="7"/>
       <c r="C113" s="7"/>
     </row>
-    <row r="114" spans="2:4" s="4" customFormat="1" ht="26.25">
-      <c r="D114" s="5" t="s">
+    <row r="114" spans="2:4" s="6" customFormat="1">
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+    </row>
+    <row r="115" spans="2:4" s="6" customFormat="1">
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+    </row>
+    <row r="116" spans="2:4" s="4" customFormat="1" ht="26.25">
+      <c r="D116" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="115" spans="2:4" s="3" customFormat="1"/>
-    <row r="116" spans="2:4" s="3" customFormat="1"/>
-    <row r="117" spans="2:4" s="4" customFormat="1" ht="26.25">
-      <c r="D117" s="5" t="s">
+    <row r="117" spans="2:4" s="3" customFormat="1"/>
+    <row r="118" spans="2:4" s="3" customFormat="1"/>
+    <row r="119" spans="2:4" s="4" customFormat="1" ht="26.25">
+      <c r="D119" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="118" spans="2:4" s="2" customFormat="1">
-      <c r="D118" s="2" t="s">
+    <row r="120" spans="2:4" s="2" customFormat="1">
+      <c r="D120" s="2" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" s="2" customFormat="1">
-      <c r="D119" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" s="2" customFormat="1">
-      <c r="C120" s="15"/>
-      <c r="D120" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="121" spans="2:4" s="2" customFormat="1">
       <c r="D121" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" s="2" customFormat="1">
+      <c r="C122" s="15"/>
+      <c r="D122" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" s="2" customFormat="1">
+      <c r="D123" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="2:4" s="2" customFormat="1">
-      <c r="D122" s="2" t="s">
+    <row r="124" spans="2:4" s="2" customFormat="1">
+      <c r="D124" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="123" spans="2:4" s="2" customFormat="1"/>
-    <row r="124" spans="2:4" s="2" customFormat="1"/>
     <row r="125" spans="2:4" s="2" customFormat="1"/>
-    <row r="126" spans="2:4" s="3" customFormat="1"/>
-    <row r="127" spans="2:4" s="3" customFormat="1"/>
-    <row r="128" spans="2:4" s="4" customFormat="1" ht="26.25">
-      <c r="D128" s="5" t="s">
+    <row r="126" spans="2:4" s="2" customFormat="1"/>
+    <row r="127" spans="2:4" s="2" customFormat="1"/>
+    <row r="128" spans="2:4" s="3" customFormat="1"/>
+    <row r="129" spans="4:4" s="3" customFormat="1"/>
+    <row r="130" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D130" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="129" spans="4:4" s="10" customFormat="1">
-      <c r="D129" s="10" t="s">
+    <row r="131" spans="4:4" s="10" customFormat="1">
+      <c r="D131" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="4:4" s="3" customFormat="1"/>
-    <row r="131" spans="4:4" s="3" customFormat="1"/>
-    <row r="132" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D132" s="5" t="s">
+    <row r="132" spans="4:4" s="3" customFormat="1"/>
+    <row r="133" spans="4:4" s="3" customFormat="1"/>
+    <row r="134" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D134" s="5" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="133" spans="4:4" s="9" customFormat="1">
-      <c r="D133" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="134" spans="4:4" s="9" customFormat="1">
-      <c r="D134" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="135" spans="4:4" s="9" customFormat="1">
       <c r="D135" s="9" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
     </row>
     <row r="136" spans="4:4" s="9" customFormat="1">
       <c r="D136" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" s="9" customFormat="1">
+      <c r="D137" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" s="9" customFormat="1">
+      <c r="D138" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="4:4" s="3" customFormat="1"/>
-    <row r="138" spans="4:4" s="3" customFormat="1"/>
-    <row r="139" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D139" s="5" t="s">
+    <row r="139" spans="4:4" s="3" customFormat="1"/>
+    <row r="140" spans="4:4" s="3" customFormat="1"/>
+    <row r="141" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D141" s="5" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="140" spans="4:4" s="11" customFormat="1">
-      <c r="D140" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="141" spans="4:4" s="11" customFormat="1">
-      <c r="D141" s="11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="142" spans="4:4" s="11" customFormat="1">
       <c r="D142" s="11" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="143" spans="4:4" s="11" customFormat="1">
       <c r="D143" s="11" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" spans="4:4" s="11" customFormat="1">
       <c r="D144" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" spans="4:4" s="11" customFormat="1">
       <c r="D145" s="11" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="146" spans="4:4" s="11" customFormat="1">
       <c r="D146" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="147" spans="4:4" s="11" customFormat="1">
       <c r="D147" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="4:4" s="11" customFormat="1">
       <c r="D148" s="11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149" spans="4:4" s="11" customFormat="1">
       <c r="D149" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="4:4" s="11" customFormat="1">
       <c r="D150" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="151" spans="4:4" s="16" customFormat="1">
-      <c r="D151" s="16" t="s">
-        <v>107</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" s="11" customFormat="1">
+      <c r="D151" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="152" spans="4:4" s="11" customFormat="1">
       <c r="D152" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="153" spans="4:4" s="11" customFormat="1">
-      <c r="D153" s="11" t="s">
-        <v>91</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" s="16" customFormat="1">
+      <c r="D153" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="154" spans="4:4" s="11" customFormat="1">
       <c r="D154" s="11" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="155" spans="4:4" s="11" customFormat="1">
       <c r="D155" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" s="11" customFormat="1">
+      <c r="D156" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" s="11" customFormat="1">
+      <c r="D157" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="156" spans="4:4" s="3" customFormat="1"/>
-    <row r="157" spans="4:4" s="3" customFormat="1"/>
+    <row r="158" spans="4:4" s="3" customFormat="1"/>
+    <row r="159" spans="4:4" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>

</xml_diff>

<commit_message>
updated art again whee
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="158">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>add tutorial popup state</t>
+  </si>
+  <si>
+    <t>enter on player name entry etc</t>
+  </si>
+  <si>
+    <t>help screen pages 2 and 3 need to work again (tiles)</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +581,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -603,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -621,6 +633,8 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K375"/>
+  <dimension ref="A1:K371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2602,8 +2616,19 @@
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="1:4" s="6" customFormat="1">
-      <c r="C121" s="7"/>
+    <row r="121" spans="1:4" s="17" customFormat="1">
+      <c r="A121" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" s="18">
+        <v>39965</v>
+      </c>
+      <c r="D121" s="17" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="122" spans="1:4" s="6" customFormat="1">
       <c r="C122" s="7"/>
@@ -2611,129 +2636,121 @@
     <row r="123" spans="1:4" s="6" customFormat="1">
       <c r="C123" s="7"/>
     </row>
-    <row r="124" spans="1:4" s="6" customFormat="1">
-      <c r="C124" s="7"/>
-    </row>
-    <row r="125" spans="1:4" s="6" customFormat="1">
-      <c r="C125" s="7"/>
-    </row>
-    <row r="126" spans="1:4" s="6" customFormat="1">
-      <c r="C126" s="7"/>
-    </row>
-    <row r="127" spans="1:4" s="6" customFormat="1">
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-    </row>
-    <row r="128" spans="1:4" s="6" customFormat="1">
-      <c r="B128" s="7"/>
-      <c r="C128" s="7"/>
-    </row>
+    <row r="124" spans="1:4" s="3" customFormat="1"/>
+    <row r="125" spans="1:4" s="3" customFormat="1"/>
+    <row r="126" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D126" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" s="3" customFormat="1"/>
+    <row r="128" spans="1:4" s="3" customFormat="1"/>
     <row r="129" spans="3:4" s="4" customFormat="1" ht="26.25">
       <c r="D129" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="130" spans="3:4" s="3" customFormat="1"/>
-    <row r="131" spans="3:4" s="3" customFormat="1"/>
-    <row r="132" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D132" s="5" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4" s="2" customFormat="1">
+      <c r="D130" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="131" spans="3:4" s="2" customFormat="1">
+      <c r="D131" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="132" spans="3:4" s="2" customFormat="1">
+      <c r="C132" s="15"/>
+      <c r="D132" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="133" spans="3:4" s="2" customFormat="1">
       <c r="D133" s="2" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="3:4" s="2" customFormat="1">
+      <c r="C134" s="15"/>
       <c r="D134" s="2" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="3:4" s="2" customFormat="1">
-      <c r="C135" s="15"/>
       <c r="D135" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="136" spans="3:4" s="2" customFormat="1">
-      <c r="D136" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="137" spans="3:4" s="2" customFormat="1">
-      <c r="C137" s="15"/>
-      <c r="D137" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="138" spans="3:4" s="2" customFormat="1"/>
-    <row r="139" spans="3:4" s="2" customFormat="1"/>
-    <row r="140" spans="3:4" s="2" customFormat="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136" spans="3:4" s="2" customFormat="1"/>
+    <row r="137" spans="3:4" s="3" customFormat="1"/>
+    <row r="138" spans="3:4" s="3" customFormat="1"/>
+    <row r="139" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D139" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="3:4" s="10" customFormat="1">
+      <c r="D140" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="141" spans="3:4" s="3" customFormat="1"/>
     <row r="142" spans="3:4" s="3" customFormat="1"/>
     <row r="143" spans="3:4" s="4" customFormat="1" ht="26.25">
       <c r="D143" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="144" spans="3:4" s="10" customFormat="1">
-      <c r="D144" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="145" spans="4:4" s="3" customFormat="1"/>
-    <row r="146" spans="4:4" s="3" customFormat="1"/>
-    <row r="147" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D147" s="5" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" s="11" customFormat="1">
+      <c r="D144" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" s="11" customFormat="1">
+      <c r="D145" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" s="11" customFormat="1">
+      <c r="D146" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" s="11" customFormat="1">
+      <c r="D147" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="4:4" s="11" customFormat="1">
       <c r="D148" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="149" spans="4:4" s="11" customFormat="1">
-      <c r="D149" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" s="16" customFormat="1">
+      <c r="D149" s="16" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="4:4" s="11" customFormat="1">
       <c r="D150" s="11" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="151" spans="4:4" s="11" customFormat="1">
       <c r="D151" s="11" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
     </row>
     <row r="152" spans="4:4" s="11" customFormat="1">
       <c r="D152" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="153" spans="4:4" s="16" customFormat="1">
-      <c r="D153" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="154" spans="4:4" s="11" customFormat="1">
-      <c r="D154" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="155" spans="4:4" s="11" customFormat="1">
-      <c r="D155" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="156" spans="4:4" s="11" customFormat="1">
-      <c r="D156" s="11" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="153" spans="4:4" s="3" customFormat="1"/>
+    <row r="154" spans="4:4" s="3" customFormat="1"/>
+    <row r="155" spans="4:4" s="3" customFormat="1"/>
+    <row r="156" spans="4:4" s="3" customFormat="1"/>
     <row r="157" spans="4:4" s="3" customFormat="1"/>
     <row r="158" spans="4:4" s="3" customFormat="1"/>
     <row r="159" spans="4:4" s="3" customFormat="1"/>
@@ -2949,10 +2966,6 @@
     <row r="369" s="3" customFormat="1"/>
     <row r="370" s="3" customFormat="1"/>
     <row r="371" s="3" customFormat="1"/>
-    <row r="372" s="3" customFormat="1"/>
-    <row r="373" s="3" customFormat="1"/>
-    <row r="374" s="3" customFormat="1"/>
-    <row r="375" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>

</xml_diff>

<commit_message>
jump animations are 1/3 faster processing of switches/dswitches are 4x faster than your process speed execute doesn't reset the map rotation anymore reprogram popup text is green now and repositioned dswitches now support tutorial tiles tutorial tile art is in the game jumping down to the left layering is fixed draw heights of climb tiles fixed switches once again switch their art regardless of if it points to a switch in code
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="170">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -490,6 +490,42 @@
   </si>
   <si>
     <t>help screen pages 2 and 3 need to work again (tiles)</t>
+  </si>
+  <si>
+    <t>repgrogram text needs to be green and in the proper location</t>
+  </si>
+  <si>
+    <t>fix draw heights of climb tiles</t>
+  </si>
+  <si>
+    <t>Level Name</t>
+  </si>
+  <si>
+    <t>Mouse Trap</t>
+  </si>
+  <si>
+    <t>Memory Used</t>
+  </si>
+  <si>
+    <t>switches need to switch its self art to inactive even if there is no code attached to it</t>
+  </si>
+  <si>
+    <t>jumping down to left needs an extra +1 y or just a +1 overall, not sure, try jumping on mousetrap level right at the start</t>
+  </si>
+  <si>
+    <t>execute needs to not reset the map's rotation</t>
+  </si>
+  <si>
+    <t>landing a jump on a tutorial square breaks shit</t>
+  </si>
+  <si>
+    <t>processing switches/dswitches should process at 4x speed of your processing speed</t>
+  </si>
+  <si>
+    <t>dswitches need to support a 41st tile</t>
+  </si>
+  <si>
+    <t>speed up jump animations</t>
   </si>
 </sst>
 </file>
@@ -520,7 +556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,12 +617,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -615,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -633,8 +663,6 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K371"/>
+  <dimension ref="A1:K389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:XFD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2616,161 +2644,290 @@
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="1:4" s="17" customFormat="1">
-      <c r="A121" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B121" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C121" s="18">
+    <row r="121" spans="1:4" s="6" customFormat="1">
+      <c r="A121" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" s="7">
         <v>39965</v>
       </c>
-      <c r="D121" s="17" t="s">
+      <c r="D121" s="6" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="6" customFormat="1">
-      <c r="C122" s="7"/>
+      <c r="A122" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C122" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="123" spans="1:4" s="6" customFormat="1">
-      <c r="C123" s="7"/>
-    </row>
-    <row r="124" spans="1:4" s="3" customFormat="1"/>
-    <row r="125" spans="1:4" s="3" customFormat="1"/>
-    <row r="126" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D126" s="5" t="s">
+      <c r="A123" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" s="6" customFormat="1">
+      <c r="A124" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C124" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" s="6" customFormat="1">
+      <c r="A125" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" s="6" customFormat="1">
+      <c r="A126" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" s="6" customFormat="1">
+      <c r="A127" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" s="6" customFormat="1">
+      <c r="A128" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C128" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" s="6" customFormat="1">
+      <c r="A129" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" s="6" customFormat="1">
+      <c r="A130" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C130" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" s="6" customFormat="1">
+      <c r="C131" s="7"/>
+    </row>
+    <row r="132" spans="1:4" s="6" customFormat="1">
+      <c r="C132" s="7"/>
+    </row>
+    <row r="133" spans="1:4" s="6" customFormat="1">
+      <c r="C133" s="7"/>
+    </row>
+    <row r="134" spans="1:4" s="6" customFormat="1">
+      <c r="C134" s="7"/>
+    </row>
+    <row r="135" spans="1:4" s="6" customFormat="1">
+      <c r="C135" s="7"/>
+    </row>
+    <row r="136" spans="1:4" s="6" customFormat="1">
+      <c r="C136" s="7"/>
+    </row>
+    <row r="137" spans="1:4" s="6" customFormat="1">
+      <c r="C137" s="7"/>
+    </row>
+    <row r="138" spans="1:4" s="6" customFormat="1">
+      <c r="C138" s="7"/>
+    </row>
+    <row r="139" spans="1:4" s="3" customFormat="1"/>
+    <row r="140" spans="1:4" s="3" customFormat="1"/>
+    <row r="141" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D141" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="127" spans="1:4" s="3" customFormat="1"/>
-    <row r="128" spans="1:4" s="3" customFormat="1"/>
-    <row r="129" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D129" s="5" t="s">
+    <row r="142" spans="1:4" s="3" customFormat="1"/>
+    <row r="143" spans="1:4" s="3" customFormat="1"/>
+    <row r="144" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D144" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="3:4" s="2" customFormat="1">
-      <c r="D130" s="2" t="s">
+    <row r="145" spans="3:4" s="2" customFormat="1">
+      <c r="D145" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="131" spans="3:4" s="2" customFormat="1">
-      <c r="D131" s="2" t="s">
+    <row r="146" spans="3:4" s="2" customFormat="1">
+      <c r="D146" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="132" spans="3:4" s="2" customFormat="1">
-      <c r="C132" s="15"/>
-      <c r="D132" s="2" t="s">
+    <row r="147" spans="3:4" s="2" customFormat="1">
+      <c r="C147" s="15"/>
+      <c r="D147" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="3:4" s="2" customFormat="1">
-      <c r="D133" s="2" t="s">
+    <row r="148" spans="3:4" s="2" customFormat="1">
+      <c r="D148" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="134" spans="3:4" s="2" customFormat="1">
-      <c r="C134" s="15"/>
-      <c r="D134" s="2" t="s">
+    <row r="149" spans="3:4" s="2" customFormat="1">
+      <c r="C149" s="15"/>
+      <c r="D149" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="135" spans="3:4" s="2" customFormat="1">
-      <c r="D135" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="3:4" s="2" customFormat="1"/>
-    <row r="137" spans="3:4" s="3" customFormat="1"/>
-    <row r="138" spans="3:4" s="3" customFormat="1"/>
-    <row r="139" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D139" s="5" t="s">
+    <row r="150" spans="3:4" s="2" customFormat="1">
+      <c r="D150" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="151" spans="3:4" s="2" customFormat="1"/>
+    <row r="152" spans="3:4" s="2" customFormat="1"/>
+    <row r="153" spans="3:4" s="2" customFormat="1"/>
+    <row r="154" spans="3:4" s="2" customFormat="1"/>
+    <row r="155" spans="3:4" s="3" customFormat="1"/>
+    <row r="156" spans="3:4" s="3" customFormat="1"/>
+    <row r="157" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D157" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="3:4" s="10" customFormat="1">
-      <c r="D140" s="10" t="s">
+    <row r="158" spans="3:4" s="10" customFormat="1">
+      <c r="D158" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="141" spans="3:4" s="3" customFormat="1"/>
-    <row r="142" spans="3:4" s="3" customFormat="1"/>
-    <row r="143" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D143" s="5" t="s">
+    <row r="159" spans="3:4" s="3" customFormat="1"/>
+    <row r="160" spans="3:4" s="3" customFormat="1"/>
+    <row r="161" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D161" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="144" spans="3:4" s="11" customFormat="1">
-      <c r="D144" s="11" t="s">
+    <row r="162" spans="4:4" s="11" customFormat="1">
+      <c r="D162" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="145" spans="4:4" s="11" customFormat="1">
-      <c r="D145" s="11" t="s">
+    <row r="163" spans="4:4" s="11" customFormat="1">
+      <c r="D163" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="4:4" s="11" customFormat="1">
-      <c r="D146" s="11" t="s">
+    <row r="164" spans="4:4" s="11" customFormat="1">
+      <c r="D164" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="4:4" s="11" customFormat="1">
-      <c r="D147" s="11" t="s">
+    <row r="165" spans="4:4" s="11" customFormat="1">
+      <c r="D165" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="4:4" s="11" customFormat="1">
-      <c r="D148" s="11" t="s">
+    <row r="166" spans="4:4" s="11" customFormat="1">
+      <c r="D166" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="4:4" s="16" customFormat="1">
-      <c r="D149" s="16" t="s">
+    <row r="167" spans="4:4" s="16" customFormat="1">
+      <c r="D167" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="150" spans="4:4" s="11" customFormat="1">
-      <c r="D150" s="11" t="s">
+    <row r="168" spans="4:4" s="11" customFormat="1">
+      <c r="D168" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="4:4" s="11" customFormat="1">
-      <c r="D151" s="11" t="s">
+    <row r="169" spans="4:4" s="11" customFormat="1">
+      <c r="D169" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="152" spans="4:4" s="11" customFormat="1">
-      <c r="D152" s="11" t="s">
+    <row r="170" spans="4:4" s="11" customFormat="1">
+      <c r="D170" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="153" spans="4:4" s="3" customFormat="1"/>
-    <row r="154" spans="4:4" s="3" customFormat="1"/>
-    <row r="155" spans="4:4" s="3" customFormat="1"/>
-    <row r="156" spans="4:4" s="3" customFormat="1"/>
-    <row r="157" spans="4:4" s="3" customFormat="1"/>
-    <row r="158" spans="4:4" s="3" customFormat="1"/>
-    <row r="159" spans="4:4" s="3" customFormat="1"/>
-    <row r="160" spans="4:4" s="3" customFormat="1"/>
-    <row r="161" s="3" customFormat="1"/>
-    <row r="162" s="3" customFormat="1"/>
-    <row r="163" s="3" customFormat="1"/>
-    <row r="164" s="3" customFormat="1"/>
-    <row r="165" s="3" customFormat="1"/>
-    <row r="166" s="3" customFormat="1"/>
-    <row r="167" s="3" customFormat="1"/>
-    <row r="168" s="3" customFormat="1"/>
-    <row r="169" s="3" customFormat="1"/>
-    <row r="170" s="3" customFormat="1"/>
-    <row r="171" s="3" customFormat="1"/>
-    <row r="172" s="3" customFormat="1"/>
-    <row r="173" s="3" customFormat="1"/>
-    <row r="174" s="3" customFormat="1"/>
-    <row r="175" s="3" customFormat="1"/>
-    <row r="176" s="3" customFormat="1"/>
+    <row r="171" spans="4:4" s="3" customFormat="1"/>
+    <row r="172" spans="4:4" s="3" customFormat="1"/>
+    <row r="173" spans="4:4" s="3" customFormat="1"/>
+    <row r="174" spans="4:4" s="3" customFormat="1"/>
+    <row r="175" spans="4:4" s="3" customFormat="1"/>
+    <row r="176" spans="4:4" s="3" customFormat="1"/>
     <row r="177" s="3" customFormat="1"/>
     <row r="178" s="3" customFormat="1"/>
     <row r="179" s="3" customFormat="1"/>
@@ -2966,6 +3123,24 @@
     <row r="369" s="3" customFormat="1"/>
     <row r="370" s="3" customFormat="1"/>
     <row r="371" s="3" customFormat="1"/>
+    <row r="372" s="3" customFormat="1"/>
+    <row r="373" s="3" customFormat="1"/>
+    <row r="374" s="3" customFormat="1"/>
+    <row r="375" s="3" customFormat="1"/>
+    <row r="376" s="3" customFormat="1"/>
+    <row r="377" s="3" customFormat="1"/>
+    <row r="378" s="3" customFormat="1"/>
+    <row r="379" s="3" customFormat="1"/>
+    <row r="380" s="3" customFormat="1"/>
+    <row r="381" s="3" customFormat="1"/>
+    <row r="382" s="3" customFormat="1"/>
+    <row r="383" s="3" customFormat="1"/>
+    <row r="384" s="3" customFormat="1"/>
+    <row r="385" s="3" customFormat="1"/>
+    <row r="386" s="3" customFormat="1"/>
+    <row r="387" s="3" customFormat="1"/>
+    <row r="388" s="3" customFormat="1"/>
+    <row r="389" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>
@@ -2977,14 +3152,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="A1:K21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
switches slowed again rotation fixed (hopefully) for execution
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="wish list" sheetId="1" r:id="rId1"/>
+    <sheet name="level notes" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="175">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -526,6 +526,21 @@
   </si>
   <si>
     <t>speed up jump animations</t>
+  </si>
+  <si>
+    <t>Oscar 6</t>
+  </si>
+  <si>
+    <t>CANNOT BEAT LEVEL</t>
+  </si>
+  <si>
+    <t>Oscar 7</t>
+  </si>
+  <si>
+    <t>make switches slower again</t>
+  </si>
+  <si>
+    <t>Oscar 8</t>
   </si>
 </sst>
 </file>
@@ -957,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K389"/>
+  <dimension ref="A1:K388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:XFD130"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2753,7 +2768,7 @@
         <v>39965</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:4" s="6" customFormat="1">
@@ -2767,7 +2782,7 @@
         <v>39965</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:4" s="6" customFormat="1">
@@ -2781,11 +2796,22 @@
         <v>39965</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="6" customFormat="1">
-      <c r="C131" s="7"/>
+      <c r="A131" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C131" s="7">
+        <v>39965</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="132" spans="1:4" s="6" customFormat="1">
       <c r="C132" s="7"/>
@@ -2808,120 +2834,122 @@
     <row r="138" spans="1:4" s="6" customFormat="1">
       <c r="C138" s="7"/>
     </row>
-    <row r="139" spans="1:4" s="3" customFormat="1"/>
+    <row r="139" spans="1:4" s="6" customFormat="1">
+      <c r="C139" s="7"/>
+    </row>
     <row r="140" spans="1:4" s="3" customFormat="1"/>
-    <row r="141" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D141" s="5" t="s">
+    <row r="141" spans="1:4" s="3" customFormat="1"/>
+    <row r="142" spans="1:4" s="4" customFormat="1" ht="26.25">
+      <c r="D142" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="3" customFormat="1"/>
     <row r="143" spans="1:4" s="3" customFormat="1"/>
-    <row r="144" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D144" s="5" t="s">
+    <row r="144" spans="1:4" s="3" customFormat="1"/>
+    <row r="145" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D145" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="145" spans="3:4" s="2" customFormat="1">
-      <c r="D145" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="146" spans="3:4" s="2" customFormat="1">
       <c r="D146" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="3:4" s="2" customFormat="1">
+      <c r="D147" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="147" spans="3:4" s="2" customFormat="1">
-      <c r="C147" s="15"/>
-      <c r="D147" s="2" t="s">
+    <row r="148" spans="3:4" s="2" customFormat="1">
+      <c r="C148" s="15"/>
+      <c r="D148" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="148" spans="3:4" s="2" customFormat="1">
-      <c r="D148" s="2" t="s">
+    <row r="149" spans="3:4" s="2" customFormat="1">
+      <c r="D149" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="149" spans="3:4" s="2" customFormat="1">
-      <c r="C149" s="15"/>
-      <c r="D149" s="2" t="s">
+    <row r="150" spans="3:4" s="2" customFormat="1">
+      <c r="C150" s="15"/>
+      <c r="D150" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="150" spans="3:4" s="2" customFormat="1">
-      <c r="D150" s="2" t="s">
+    <row r="151" spans="3:4" s="2" customFormat="1">
+      <c r="D151" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="151" spans="3:4" s="2" customFormat="1"/>
     <row r="152" spans="3:4" s="2" customFormat="1"/>
     <row r="153" spans="3:4" s="2" customFormat="1"/>
-    <row r="154" spans="3:4" s="2" customFormat="1"/>
+    <row r="154" spans="3:4" s="3" customFormat="1"/>
     <row r="155" spans="3:4" s="3" customFormat="1"/>
-    <row r="156" spans="3:4" s="3" customFormat="1"/>
-    <row r="157" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D157" s="5" t="s">
+    <row r="156" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D156" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="158" spans="3:4" s="10" customFormat="1">
-      <c r="D158" s="10" t="s">
+    <row r="157" spans="3:4" s="10" customFormat="1">
+      <c r="D157" s="10" t="s">
         <v>149</v>
       </c>
     </row>
+    <row r="158" spans="3:4" s="3" customFormat="1"/>
     <row r="159" spans="3:4" s="3" customFormat="1"/>
-    <row r="160" spans="3:4" s="3" customFormat="1"/>
-    <row r="161" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D161" s="5" t="s">
+    <row r="160" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D160" s="5" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" s="11" customFormat="1">
+      <c r="D161" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="162" spans="4:4" s="11" customFormat="1">
       <c r="D162" s="11" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="4:4" s="11" customFormat="1">
       <c r="D163" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="164" spans="4:4" s="11" customFormat="1">
       <c r="D164" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="4:4" s="11" customFormat="1">
       <c r="D165" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="166" spans="4:4" s="11" customFormat="1">
-      <c r="D166" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="4:4" s="16" customFormat="1">
-      <c r="D167" s="16" t="s">
+    <row r="166" spans="4:4" s="16" customFormat="1">
+      <c r="D166" s="16" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" s="11" customFormat="1">
+      <c r="D167" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="168" spans="4:4" s="11" customFormat="1">
       <c r="D168" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="169" spans="4:4" s="11" customFormat="1">
       <c r="D169" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="170" spans="4:4" s="11" customFormat="1">
-      <c r="D170" s="11" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="170" spans="4:4" s="3" customFormat="1"/>
     <row r="171" spans="4:4" s="3" customFormat="1"/>
     <row r="172" spans="4:4" s="3" customFormat="1"/>
     <row r="173" spans="4:4" s="3" customFormat="1"/>
@@ -3140,7 +3168,6 @@
     <row r="386" s="3" customFormat="1"/>
     <row r="387" s="3" customFormat="1"/>
     <row r="388" s="3" customFormat="1"/>
-    <row r="389" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>
@@ -3152,10 +3179,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C3"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3177,6 +3204,30 @@
       </c>
       <c r="C3">
         <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zoom resets after you click "you died" movieclip oscar maps 8 9 10 are now balanced
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wish list" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="178">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>Oscar 8</t>
+  </si>
+  <si>
+    <t>Oscar 9</t>
+  </si>
+  <si>
+    <t>when you click the you died window, make it reset zoom to default</t>
+  </si>
+  <si>
+    <t>Oscar 10</t>
   </si>
 </sst>
 </file>
@@ -972,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K388"/>
+  <dimension ref="A1:K389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2883,73 +2892,77 @@
         <v>166</v>
       </c>
     </row>
-    <row r="152" spans="3:4" s="2" customFormat="1"/>
+    <row r="152" spans="3:4" s="2" customFormat="1">
+      <c r="D152" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
     <row r="153" spans="3:4" s="2" customFormat="1"/>
-    <row r="154" spans="3:4" s="3" customFormat="1"/>
+    <row r="154" spans="3:4" s="2" customFormat="1"/>
     <row r="155" spans="3:4" s="3" customFormat="1"/>
-    <row r="156" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D156" s="5" t="s">
+    <row r="156" spans="3:4" s="3" customFormat="1"/>
+    <row r="157" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D157" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="157" spans="3:4" s="10" customFormat="1">
-      <c r="D157" s="10" t="s">
+    <row r="158" spans="3:4" s="10" customFormat="1">
+      <c r="D158" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="3:4" s="3" customFormat="1"/>
     <row r="159" spans="3:4" s="3" customFormat="1"/>
-    <row r="160" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D160" s="5" t="s">
+    <row r="160" spans="3:4" s="3" customFormat="1"/>
+    <row r="161" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D161" s="5" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="161" spans="4:4" s="11" customFormat="1">
-      <c r="D161" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="162" spans="4:4" s="11" customFormat="1">
       <c r="D162" s="11" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="163" spans="4:4" s="11" customFormat="1">
       <c r="D163" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="4:4" s="11" customFormat="1">
       <c r="D164" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="165" spans="4:4" s="11" customFormat="1">
       <c r="D165" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" s="11" customFormat="1">
+      <c r="D166" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="4:4" s="16" customFormat="1">
-      <c r="D166" s="16" t="s">
+    <row r="167" spans="4:4" s="16" customFormat="1">
+      <c r="D167" s="16" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="167" spans="4:4" s="11" customFormat="1">
-      <c r="D167" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="168" spans="4:4" s="11" customFormat="1">
       <c r="D168" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="169" spans="4:4" s="11" customFormat="1">
       <c r="D169" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" s="11" customFormat="1">
+      <c r="D170" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="170" spans="4:4" s="3" customFormat="1"/>
     <row r="171" spans="4:4" s="3" customFormat="1"/>
     <row r="172" spans="4:4" s="3" customFormat="1"/>
     <row r="173" spans="4:4" s="3" customFormat="1"/>
@@ -3168,6 +3181,7 @@
     <row r="386" s="3" customFormat="1"/>
     <row r="387" s="3" customFormat="1"/>
     <row r="388" s="3" customFormat="1"/>
+    <row r="389" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>
@@ -3179,10 +3193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3228,6 +3242,22 @@
       </c>
       <c r="C12">
         <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trace removals - more to come
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="183">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>for final release - make sure level select is clamped</t>
+  </si>
+  <si>
+    <t>new as of 6/2/2009</t>
+  </si>
+  <si>
+    <t>all instructions are appearing at the top left corner for a moment, probably due to skip this tutorial button skipping immediately into the next level without going to pregame</t>
+  </si>
+  <si>
+    <t>skip this tutorial button needs to fire into next level's pregame</t>
+  </si>
+  <si>
+    <t>during death animation - getting an error "cannot access a property or method of a null object reference inside of processRobot()</t>
   </si>
 </sst>
 </file>
@@ -986,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K395"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2906,11 +2918,27 @@
       </c>
     </row>
     <row r="154" spans="3:4" s="2" customFormat="1"/>
-    <row r="155" spans="3:4" s="2" customFormat="1"/>
-    <row r="156" spans="3:4" s="2" customFormat="1"/>
-    <row r="157" spans="3:4" s="2" customFormat="1"/>
+    <row r="155" spans="3:4" s="2" customFormat="1">
+      <c r="D155" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="156" spans="3:4" s="2" customFormat="1">
+      <c r="D156" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="157" spans="3:4" s="2" customFormat="1">
+      <c r="D157" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="158" spans="3:4" s="2" customFormat="1"/>
-    <row r="159" spans="3:4" s="2" customFormat="1"/>
+    <row r="159" spans="3:4" s="2" customFormat="1">
+      <c r="D159" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
     <row r="160" spans="3:4" s="2" customFormat="1"/>
     <row r="161" spans="4:4" s="3" customFormat="1"/>
     <row r="162" spans="4:4" s="3" customFormat="1"/>
@@ -3209,7 +3237,7 @@
   <dimension ref="A2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added new button "info" for corwin to hook up to making the tutorial info pop up manually added "skip level" button to top right of screen made skip tutorial button and info button vanish once you are past a tutorial level various animation and teleporter fixes error in trace window for when teleporters have no attached code for them (i.e. teleporter will not work right) added error sound for bad teleporters
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="191">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -60,18 +60,12 @@
     <t>text for tiles needs to be added</t>
   </si>
   <si>
-    <t>hovers for tiles needs to be added</t>
-  </si>
-  <si>
     <t>click on a tile should launch a popup window thing showing an animation of that tile being used</t>
   </si>
   <si>
     <t>instructions need description</t>
   </si>
   <si>
-    <t>hover for instructions needs to be added</t>
-  </si>
-  <si>
     <t>click on an instruction should launch a popup window thing showing an animation of that instruction being used</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>multiple boards are being loaded/etc from level select stuff</t>
   </si>
   <si>
-    <t>"sometimes" teleporters aren't firing properly, really hard to reproduce</t>
-  </si>
-  <si>
     <t>subroutines need to work</t>
   </si>
   <si>
@@ -555,16 +546,49 @@
     <t>for final release - make sure level select is clamped</t>
   </si>
   <si>
-    <t>new as of 6/2/2009</t>
-  </si>
-  <si>
-    <t>all instructions are appearing at the top left corner for a moment, probably due to skip this tutorial button skipping immediately into the next level without going to pregame</t>
-  </si>
-  <si>
-    <t>skip this tutorial button needs to fire into next level's pregame</t>
-  </si>
-  <si>
-    <t>during death animation - getting an error "cannot access a property or method of a null object reference inside of processRobot()</t>
+    <t>as soon as tutorial level pops up, getting an error in tutorialtilecheckandexecution() - needed to wait for the level to finish loading</t>
+  </si>
+  <si>
+    <t>new help page - tutorial movieclip</t>
+  </si>
+  <si>
+    <t>once death animation starts running, need to clear out all ui abilities until clicking ok on you died</t>
+  </si>
+  <si>
+    <t>upon arrival from a teleport, robot needs to reinject</t>
+  </si>
+  <si>
+    <t>add error checking for teleporters to make sure that there is an assigned bit of teleport code for it, if not, trace out an error</t>
+  </si>
+  <si>
+    <t>logic interface should not let you click and drag thingies when it says "you died" on the screen</t>
+  </si>
+  <si>
+    <t>TUTORIAL - ability to go backwards in the text reader thingie to see old tutorial info</t>
+  </si>
+  <si>
+    <t>TUTORIAL - don’t' let them scroll too far etc</t>
+  </si>
+  <si>
+    <t>TUTORIAL - button to bring up tutorial text at any time for current status of tutorial progress</t>
+  </si>
+  <si>
+    <t>maps need tobe reordered</t>
+  </si>
+  <si>
+    <t>maybe include maps inside the swf once they are finalized</t>
+  </si>
+  <si>
+    <t>victory dance</t>
+  </si>
+  <si>
+    <t>remove tutoriallevel++ from all but the real tutorial level</t>
+  </si>
+  <si>
+    <t>if I have time, make sure that all teleporters that can appear via a dswitch have associated code</t>
+  </si>
+  <si>
+    <t>make the info/skip tutorial buttons vanish when you skip past tutorials</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K395"/>
+  <dimension ref="A1:K403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1024,11 +1048,11 @@
       <c r="D1" s="8"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="26.25">
@@ -1038,16 +1062,16 @@
       <c r="D2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="26.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -1060,39 +1084,39 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1"/>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="26.25">
       <c r="D5" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="7">
         <v>39953</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="6" customFormat="1">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7">
         <v>39953</v>
@@ -1103,10 +1127,10 @@
     </row>
     <row r="8" spans="1:11" s="6" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="7">
         <v>39953</v>
@@ -1117,10 +1141,10 @@
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7">
         <v>39953</v>
@@ -1131,10 +1155,10 @@
     </row>
     <row r="10" spans="1:11" s="6" customFormat="1">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7">
         <v>39953</v>
@@ -1145,164 +1169,164 @@
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1">
       <c r="A11" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="7">
         <v>39953</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="6" customFormat="1">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="7">
         <v>39953</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="7">
         <v>39953</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="7">
         <v>39953</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="7">
         <v>39953</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="7">
         <v>39953</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="6" customFormat="1">
       <c r="A17" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C17" s="7">
         <v>39953</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="6" customFormat="1">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7">
         <v>39953</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="6" customFormat="1">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="7">
         <v>39953</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="6" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="7">
         <v>39953</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="6" customFormat="1">
       <c r="A21" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="7">
         <v>39953</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="6" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="7">
         <v>39954</v>
@@ -1313,318 +1337,318 @@
     </row>
     <row r="23" spans="1:4" s="6" customFormat="1">
       <c r="A23" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="7">
         <v>39954</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="6" customFormat="1">
       <c r="A24" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" s="7">
         <v>39954</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="6" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" s="7">
         <v>39954</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="6" customFormat="1">
       <c r="A26" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" s="7">
         <v>39954</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="6" customFormat="1">
       <c r="A27" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C27" s="7">
         <v>39954</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="6" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" s="7">
         <v>39954</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="6" customFormat="1">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="7">
         <v>39955</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="6" customFormat="1">
       <c r="A30" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="7">
         <v>39955</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="6" customFormat="1">
       <c r="A31" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="7">
         <v>39955</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="6" customFormat="1">
       <c r="A32" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="7">
         <v>39955</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="6" customFormat="1">
       <c r="A33" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="7">
         <v>39955</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="6" customFormat="1">
       <c r="A34" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="7">
         <v>39955</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="6" customFormat="1">
       <c r="A35" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="7">
         <v>39955</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="6" customFormat="1">
       <c r="A36" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="7">
         <v>39955</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="6" customFormat="1">
       <c r="A37" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="7">
         <v>39955</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="6" customFormat="1">
       <c r="A38" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="7">
         <v>39955</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="6" customFormat="1">
       <c r="A39" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="7">
         <v>39955</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="13" customFormat="1">
       <c r="A40" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C40" s="7">
         <v>39955</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="6" customFormat="1">
       <c r="A41" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C41" s="7">
         <v>39955</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="6" customFormat="1">
       <c r="A42" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" s="7">
         <v>39955</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="6" customFormat="1">
       <c r="A43" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C43" s="14">
         <v>39955</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="6" customFormat="1">
       <c r="A44" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="7">
         <v>39955</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="6" customFormat="1">
       <c r="A45" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45" s="7">
         <v>39955</v>
@@ -1632,150 +1656,150 @@
     </row>
     <row r="46" spans="1:4" s="6" customFormat="1">
       <c r="A46" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C46" s="7">
         <v>39955</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="6" customFormat="1">
       <c r="A47" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" s="7">
         <v>39955</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="6" customFormat="1">
       <c r="A48" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C48" s="7">
         <v>39955</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="6" customFormat="1">
       <c r="A49" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C49" s="7">
         <v>39955</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="6" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C50" s="7">
         <v>39955</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="6" customFormat="1">
       <c r="A51" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="7">
         <v>39955</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="6" customFormat="1">
       <c r="A52" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="7">
         <v>39956</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="6" customFormat="1">
       <c r="A53" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" s="7">
         <v>39956</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="6" customFormat="1">
       <c r="A54" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C54" s="7">
         <v>39956</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="6" customFormat="1">
       <c r="A55" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C55" s="14">
         <v>39956</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="6" customFormat="1">
       <c r="A56" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C56" s="7">
         <v>39957</v>
@@ -1786,430 +1810,430 @@
     </row>
     <row r="57" spans="1:4" s="6" customFormat="1">
       <c r="A57" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C57" s="7">
         <v>39957</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="6" customFormat="1">
       <c r="A58" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C58" s="14">
         <v>39957</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="6" customFormat="1">
       <c r="A59" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C59" s="7">
         <v>39957</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="6" customFormat="1">
       <c r="A60" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C60" s="7">
         <v>39957</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="6" customFormat="1">
       <c r="A61" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C61" s="7">
         <v>39957</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="6" customFormat="1">
       <c r="A62" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C62" s="7">
         <v>39957</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="6" customFormat="1">
       <c r="A63" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C63" s="7">
         <v>39957</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="6" customFormat="1">
       <c r="A64" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C64" s="7">
         <v>39957</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="6" customFormat="1">
       <c r="A65" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C65" s="7">
         <v>39957</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="6" customFormat="1">
       <c r="A66" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C66" s="7">
         <v>39957</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="13" customFormat="1">
       <c r="A67" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" s="7">
         <v>39957</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="13" customFormat="1">
       <c r="A68" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C68" s="7">
         <v>39957</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="6" customFormat="1">
       <c r="A69" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C69" s="7">
         <v>39957</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="6" customFormat="1">
       <c r="A70" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C70" s="7">
         <v>39957</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="6" customFormat="1">
       <c r="A71" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C71" s="7">
         <v>39957</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="6" customFormat="1">
       <c r="A72" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C72" s="7">
         <v>39957</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="6" customFormat="1">
       <c r="A73" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C73" s="7">
         <v>39957</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="6" customFormat="1">
       <c r="A74" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C74" s="7">
         <v>39957</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="6" customFormat="1">
       <c r="A75" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C75" s="7">
         <v>39957</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="6" customFormat="1">
       <c r="A76" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C76" s="7">
         <v>39957</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="6" customFormat="1">
       <c r="A77" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C77" s="7">
         <v>39957</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="6" customFormat="1">
       <c r="A78" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C78" s="7">
         <v>39957</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="6" customFormat="1">
       <c r="A79" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C79" s="7">
         <v>39959</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="6" customFormat="1">
       <c r="A80" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C80" s="7">
         <v>39959</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="6" customFormat="1">
       <c r="A81" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C81" s="7">
         <v>39959</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="6" customFormat="1">
       <c r="A82" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C82" s="7">
         <v>39959</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="6" customFormat="1">
       <c r="A83" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C83" s="7">
         <v>39959</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1">
       <c r="A84" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C84" s="7">
         <v>39959</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="A85" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C85" s="7">
         <v>39961</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="6" customFormat="1">
       <c r="A86" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C86" s="7">
         <v>39962</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="6" customFormat="1">
       <c r="A87" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C87" s="7">
         <v>39964</v>
@@ -2220,10 +2244,10 @@
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1">
       <c r="A88" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C88" s="7">
         <v>39964</v>
@@ -2234,10 +2258,10 @@
     </row>
     <row r="89" spans="1:5" s="6" customFormat="1">
       <c r="A89" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C89" s="7">
         <v>39964</v>
@@ -2248,10 +2272,10 @@
     </row>
     <row r="90" spans="1:5" s="7" customFormat="1">
       <c r="A90" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C90" s="7">
         <v>39964</v>
@@ -2262,764 +2286,876 @@
     </row>
     <row r="91" spans="1:5" s="7" customFormat="1">
       <c r="A91" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C91" s="7">
         <v>39964</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="7" customFormat="1">
       <c r="A92" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C92" s="7">
         <v>39964</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1">
       <c r="A93" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C93" s="7">
         <v>39964</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="6" customFormat="1">
       <c r="A94" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C94" s="7">
         <v>39964</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="6" customFormat="1">
       <c r="A95" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C95" s="7">
         <v>39964</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="6" customFormat="1">
       <c r="A96" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C96" s="7">
         <v>39964</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="6" customFormat="1">
       <c r="A97" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C97" s="7">
         <v>39964</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="6" customFormat="1">
       <c r="A98" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C98" s="7">
         <v>39964</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="6" customFormat="1">
       <c r="A99" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C99" s="7">
         <v>39964</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="6" customFormat="1">
       <c r="A100" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C100" s="7">
         <v>39964</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="6" customFormat="1">
       <c r="A101" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C101" s="7">
         <v>39964</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="6" customFormat="1">
       <c r="A102" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C102" s="7">
         <v>39964</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="6" customFormat="1">
       <c r="A103" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C103" s="7">
         <v>39964</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="6" customFormat="1">
       <c r="A104" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C104" s="7">
         <v>39964</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="6" customFormat="1">
       <c r="A105" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C105" s="7">
         <v>39964</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="6" customFormat="1">
       <c r="A106" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C106" s="7">
         <v>39964</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="6" customFormat="1">
       <c r="A107" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C107" s="7">
         <v>39964</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="6" customFormat="1">
       <c r="A108" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C108" s="7">
         <v>39964</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="6" customFormat="1">
       <c r="A109" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C109" s="7">
         <v>39964</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="6" customFormat="1">
       <c r="A110" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C110" s="7">
         <v>39964</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="6" customFormat="1">
       <c r="A111" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C111" s="7">
         <v>39964</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="6" customFormat="1">
       <c r="A112" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C112" s="7">
         <v>39964</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="6" customFormat="1">
       <c r="A113" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C113" s="7">
         <v>39964</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="6" customFormat="1">
       <c r="A114" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C114" s="7">
         <v>39965</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="6" customFormat="1">
       <c r="A115" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C115" s="7">
         <v>39965</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="6" customFormat="1">
       <c r="A116" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C116" s="7">
         <v>39964</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="6" customFormat="1">
       <c r="A117" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C117" s="7">
         <v>39965</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="6" customFormat="1">
       <c r="A118" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C118" s="7">
         <v>39965</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="6" customFormat="1">
       <c r="A119" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C119" s="7">
         <v>39965</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:4" s="6" customFormat="1">
       <c r="A120" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C120" s="7">
         <v>39965</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="6" customFormat="1">
       <c r="A121" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C121" s="7">
         <v>39965</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="6" customFormat="1">
       <c r="A122" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C122" s="7">
         <v>39965</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123" spans="1:4" s="6" customFormat="1">
       <c r="A123" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C123" s="7">
         <v>39965</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:4" s="6" customFormat="1">
       <c r="A124" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C124" s="7">
         <v>39965</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="6" customFormat="1">
       <c r="A125" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C125" s="7">
         <v>39965</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="6" customFormat="1">
       <c r="A126" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C126" s="7">
         <v>39965</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="6" customFormat="1">
       <c r="A127" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C127" s="7">
         <v>39965</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="6" customFormat="1">
       <c r="A128" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C128" s="7">
         <v>39965</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="129" spans="1:4" s="6" customFormat="1">
       <c r="A129" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C129" s="7">
         <v>39965</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:4" s="6" customFormat="1">
       <c r="A130" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C130" s="7">
         <v>39965</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="6" customFormat="1">
       <c r="A131" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C131" s="7">
         <v>39965</v>
       </c>
       <c r="D131" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" s="6" customFormat="1">
+      <c r="A132" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C132" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" s="6" customFormat="1">
+      <c r="A133" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C133" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" s="6" customFormat="1">
+      <c r="A134" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C134" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" s="6" customFormat="1">
+      <c r="A135" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C135" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" s="6" customFormat="1">
+      <c r="A136" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C136" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" s="6" customFormat="1">
+      <c r="A137" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C137" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D137" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="132" spans="1:4" s="6" customFormat="1">
-      <c r="C132" s="7"/>
-    </row>
-    <row r="133" spans="1:4" s="6" customFormat="1">
-      <c r="C133" s="7"/>
-    </row>
-    <row r="134" spans="1:4" s="6" customFormat="1">
-      <c r="C134" s="7"/>
-    </row>
-    <row r="135" spans="1:4" s="6" customFormat="1">
-      <c r="C135" s="7"/>
-    </row>
-    <row r="136" spans="1:4" s="6" customFormat="1">
-      <c r="C136" s="7"/>
-    </row>
-    <row r="137" spans="1:4" s="6" customFormat="1">
-      <c r="C137" s="7"/>
-    </row>
     <row r="138" spans="1:4" s="6" customFormat="1">
-      <c r="C138" s="7"/>
+      <c r="A138" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C138" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="139" spans="1:4" s="6" customFormat="1">
-      <c r="C139" s="7"/>
-    </row>
-    <row r="140" spans="1:4" s="3" customFormat="1"/>
-    <row r="141" spans="1:4" s="3" customFormat="1"/>
-    <row r="142" spans="1:4" s="4" customFormat="1" ht="26.25">
-      <c r="D142" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" s="3" customFormat="1"/>
-    <row r="144" spans="1:4" s="3" customFormat="1"/>
-    <row r="145" spans="3:4" s="4" customFormat="1" ht="26.25">
-      <c r="D145" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="146" spans="3:4" s="2" customFormat="1">
-      <c r="D146" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="147" spans="3:4" s="2" customFormat="1">
-      <c r="D147" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="148" spans="3:4" s="2" customFormat="1">
-      <c r="C148" s="15"/>
-      <c r="D148" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="149" spans="3:4" s="2" customFormat="1">
-      <c r="D149" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="150" spans="3:4" s="2" customFormat="1">
-      <c r="C150" s="15"/>
-      <c r="D150" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="151" spans="3:4" s="2" customFormat="1">
-      <c r="D151" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="152" spans="3:4" s="2" customFormat="1">
-      <c r="D152" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="153" spans="3:4" s="2" customFormat="1">
-      <c r="D153" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="154" spans="3:4" s="2" customFormat="1"/>
+      <c r="A139" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C139" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" s="6" customFormat="1">
+      <c r="A140" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C140" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" s="6" customFormat="1">
+      <c r="C141" s="7"/>
+    </row>
+    <row r="142" spans="1:4" s="6" customFormat="1">
+      <c r="C142" s="7"/>
+    </row>
+    <row r="143" spans="1:4" s="6" customFormat="1">
+      <c r="C143" s="7"/>
+    </row>
+    <row r="144" spans="1:4" s="6" customFormat="1">
+      <c r="C144" s="7"/>
+    </row>
+    <row r="145" spans="3:4" s="6" customFormat="1">
+      <c r="C145" s="7"/>
+    </row>
+    <row r="146" spans="3:4" s="6" customFormat="1">
+      <c r="C146" s="7"/>
+    </row>
+    <row r="147" spans="3:4" s="6" customFormat="1">
+      <c r="C147" s="7"/>
+    </row>
+    <row r="148" spans="3:4" s="6" customFormat="1">
+      <c r="C148" s="7"/>
+    </row>
+    <row r="149" spans="3:4" s="3" customFormat="1"/>
+    <row r="150" spans="3:4" s="3" customFormat="1"/>
+    <row r="151" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D151" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="152" spans="3:4" s="3" customFormat="1"/>
+    <row r="153" spans="3:4" s="3" customFormat="1"/>
+    <row r="154" spans="3:4" s="4" customFormat="1" ht="26.25">
+      <c r="D154" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="155" spans="3:4" s="2" customFormat="1">
       <c r="D155" s="2" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="156" spans="3:4" s="2" customFormat="1">
+      <c r="C156" s="15"/>
       <c r="D156" s="2" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="3:4" s="2" customFormat="1">
       <c r="D157" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="158" spans="3:4" s="2" customFormat="1">
+      <c r="D158" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="159" spans="3:4" s="2" customFormat="1"/>
+    <row r="160" spans="3:4" s="2" customFormat="1">
+      <c r="D160" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" s="2" customFormat="1">
+      <c r="D161" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" s="2" customFormat="1">
+      <c r="D162" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" s="2" customFormat="1">
+      <c r="D163" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" s="2" customFormat="1">
+      <c r="D164" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" s="2" customFormat="1">
+      <c r="D165" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" s="2" customFormat="1">
+      <c r="D166" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="158" spans="3:4" s="2" customFormat="1"/>
-    <row r="159" spans="3:4" s="2" customFormat="1">
-      <c r="D159" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="160" spans="3:4" s="2" customFormat="1"/>
-    <row r="161" spans="4:4" s="3" customFormat="1"/>
-    <row r="162" spans="4:4" s="3" customFormat="1"/>
-    <row r="163" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D163" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="164" spans="4:4" s="10" customFormat="1">
-      <c r="D164" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="165" spans="4:4" s="3" customFormat="1"/>
-    <row r="166" spans="4:4" s="3" customFormat="1"/>
-    <row r="167" spans="4:4" s="4" customFormat="1" ht="26.25">
-      <c r="D167" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="168" spans="4:4" s="11" customFormat="1">
-      <c r="D168" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="169" spans="4:4" s="11" customFormat="1">
-      <c r="D169" s="11" t="s">
+    <row r="167" spans="4:4" s="2" customFormat="1">
+      <c r="D167" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" s="2" customFormat="1">
+      <c r="D168" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" s="2" customFormat="1"/>
+    <row r="170" spans="4:4" s="2" customFormat="1"/>
+    <row r="171" spans="4:4" s="3" customFormat="1"/>
+    <row r="172" spans="4:4" s="3" customFormat="1"/>
+    <row r="173" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D173" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="174" spans="4:4" s="10" customFormat="1">
+      <c r="D174" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="175" spans="4:4" s="3" customFormat="1"/>
+    <row r="176" spans="4:4" s="3" customFormat="1"/>
+    <row r="177" spans="4:4" s="4" customFormat="1" ht="26.25">
+      <c r="D177" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" s="11" customFormat="1">
+      <c r="D178" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="179" spans="4:4" s="11" customFormat="1">
+      <c r="D179" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="4:4" s="11" customFormat="1">
-      <c r="D170" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="171" spans="4:4" s="11" customFormat="1">
-      <c r="D171" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="172" spans="4:4" s="11" customFormat="1">
-      <c r="D172" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="173" spans="4:4" s="16" customFormat="1">
-      <c r="D173" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="174" spans="4:4" s="11" customFormat="1">
-      <c r="D174" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="175" spans="4:4" s="11" customFormat="1">
-      <c r="D175" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="176" spans="4:4" s="11" customFormat="1">
-      <c r="D176" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="177" s="3" customFormat="1"/>
-    <row r="178" s="3" customFormat="1"/>
-    <row r="179" s="3" customFormat="1"/>
-    <row r="180" s="3" customFormat="1"/>
-    <row r="181" s="3" customFormat="1"/>
-    <row r="182" s="3" customFormat="1"/>
-    <row r="183" s="3" customFormat="1"/>
-    <row r="184" s="3" customFormat="1"/>
-    <row r="185" s="3" customFormat="1"/>
-    <row r="186" s="3" customFormat="1"/>
-    <row r="187" s="3" customFormat="1"/>
-    <row r="188" s="3" customFormat="1"/>
-    <row r="189" s="3" customFormat="1"/>
-    <row r="190" s="3" customFormat="1"/>
-    <row r="191" s="3" customFormat="1"/>
-    <row r="192" s="3" customFormat="1"/>
+    <row r="180" spans="4:4" s="6" customFormat="1">
+      <c r="D180" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="4:4" s="16" customFormat="1">
+      <c r="D181" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="182" spans="4:4" s="11" customFormat="1">
+      <c r="D182" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="183" spans="4:4" s="11" customFormat="1">
+      <c r="D183" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="184" spans="4:4" s="11" customFormat="1">
+      <c r="D184" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="185" spans="4:4" s="3" customFormat="1"/>
+    <row r="186" spans="4:4" s="3" customFormat="1"/>
+    <row r="187" spans="4:4" s="3" customFormat="1"/>
+    <row r="188" spans="4:4" s="3" customFormat="1"/>
+    <row r="189" spans="4:4" s="3" customFormat="1"/>
+    <row r="190" spans="4:4" s="3" customFormat="1"/>
+    <row r="191" spans="4:4" s="3" customFormat="1"/>
+    <row r="192" spans="4:4" s="3" customFormat="1"/>
     <row r="193" s="3" customFormat="1"/>
     <row r="194" s="3" customFormat="1"/>
     <row r="195" s="3" customFormat="1"/>
@@ -3223,6 +3359,14 @@
     <row r="393" s="3" customFormat="1"/>
     <row r="394" s="3" customFormat="1"/>
     <row r="395" s="3" customFormat="1"/>
+    <row r="396" s="3" customFormat="1"/>
+    <row r="397" s="3" customFormat="1"/>
+    <row r="398" s="3" customFormat="1"/>
+    <row r="399" s="3" customFormat="1"/>
+    <row r="400" s="3" customFormat="1"/>
+    <row r="401" s="3" customFormat="1"/>
+    <row r="402" s="3" customFormat="1"/>
+    <row r="403" s="3" customFormat="1"/>
   </sheetData>
   <sortState ref="A7:D107">
     <sortCondition ref="C7:C107"/>
@@ -3247,15 +3391,15 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C3">
         <v>72</v>
@@ -3263,23 +3407,23 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C12">
         <v>228</v>
@@ -3287,7 +3431,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C13">
         <v>318</v>
@@ -3295,7 +3439,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C14">
         <v>156</v>

</xml_diff>

<commit_message>
Changed the positioning of the Tutorial pop ups.
Made it so the player can't click on the interface elements during a tutorial pop up or a "you died" pop up.

Made Misc. fixes to the FLA regarding tutorial pop ups.

Exported infoButton for actionscript use.
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
@@ -11,12 +11,12 @@
     <sheet name="level notes" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="191">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3052,62 +3052,80 @@
         <v>184</v>
       </c>
     </row>
-    <row r="161" spans="4:4" s="2" customFormat="1">
-      <c r="D161" s="2" t="s">
+    <row r="161" spans="1:4" s="6" customFormat="1">
+      <c r="A161" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C161" s="7">
+        <v>39966</v>
+      </c>
+      <c r="D161" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="162" spans="4:4" s="2" customFormat="1">
+    <row r="162" spans="1:4" s="2" customFormat="1">
       <c r="D162" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="163" spans="4:4" s="2" customFormat="1">
+    <row r="163" spans="1:4" s="2" customFormat="1">
       <c r="D163" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="164" spans="4:4" s="2" customFormat="1">
+    <row r="164" spans="1:4" s="2" customFormat="1">
       <c r="D164" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="165" spans="4:4" s="2" customFormat="1">
+    <row r="165" spans="1:4" s="2" customFormat="1">
       <c r="D165" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="166" spans="4:4" s="2" customFormat="1">
-      <c r="D166" s="2" t="s">
+    <row r="166" spans="1:4" s="6" customFormat="1">
+      <c r="A166" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C166" s="7">
+        <v>39967</v>
+      </c>
+      <c r="D166" s="6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="167" spans="4:4" s="2" customFormat="1">
+    <row r="167" spans="1:4" s="2" customFormat="1">
       <c r="D167" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="168" spans="4:4" s="2" customFormat="1">
+    <row r="168" spans="1:4" s="2" customFormat="1">
       <c r="D168" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="169" spans="4:4" s="2" customFormat="1"/>
-    <row r="170" spans="4:4" s="2" customFormat="1"/>
-    <row r="171" spans="4:4" s="3" customFormat="1"/>
-    <row r="172" spans="4:4" s="3" customFormat="1"/>
-    <row r="173" spans="4:4" s="4" customFormat="1" ht="26.25">
+    <row r="169" spans="1:4" s="2" customFormat="1"/>
+    <row r="170" spans="1:4" s="2" customFormat="1"/>
+    <row r="171" spans="1:4" s="3" customFormat="1"/>
+    <row r="172" spans="1:4" s="3" customFormat="1"/>
+    <row r="173" spans="1:4" s="4" customFormat="1" ht="26.25">
       <c r="D173" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="174" spans="4:4" s="10" customFormat="1">
+    <row r="174" spans="1:4" s="10" customFormat="1">
       <c r="D174" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="175" spans="4:4" s="3" customFormat="1"/>
-    <row r="176" spans="4:4" s="3" customFormat="1"/>
+    <row r="175" spans="1:4" s="3" customFormat="1"/>
+    <row r="176" spans="1:4" s="3" customFormat="1"/>
     <row r="177" spans="4:4" s="4" customFormat="1" ht="26.25">
       <c r="D177" s="5" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
flash updates, credits updates, credits embedded in flash file now, prelim for map embeds
</commit_message>
<xml_diff>
--- a/STUPID ROBOT FLASH WISH LIST.xlsx
+++ b/STUPID ROBOT FLASH WISH LIST.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="201">
   <si>
     <t>Stupid Robot Flash Wish List</t>
   </si>
@@ -566,9 +566,6 @@
     <t>maps need tobe reordered</t>
   </si>
   <si>
-    <t>maybe include maps inside the swf once they are finalized</t>
-  </si>
-  <si>
     <t>victory dance</t>
   </si>
   <si>
@@ -579,9 +576,6 @@
   </si>
   <si>
     <t>UI Diagram needs to be replaced</t>
-  </si>
-  <si>
-    <t>Sam</t>
   </si>
   <si>
     <t>Tom/Corwin</t>
@@ -3886,7 +3880,7 @@
   <dimension ref="A1:K399"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5833,7 +5827,7 @@
         <v>39966</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:4" s="6" customFormat="1">
@@ -5847,7 +5841,7 @@
         <v>39966</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="141" spans="1:4" s="6" customFormat="1">
@@ -5925,13 +5919,13 @@
         <v>54</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C146" s="7">
         <v>39971</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="147" spans="1:4" s="6" customFormat="1">
@@ -5973,7 +5967,7 @@
         <v>39971</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="150" spans="1:4" s="6" customFormat="1">
@@ -5987,7 +5981,7 @@
         <v>39971</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="151" spans="1:4" s="6" customFormat="1">
@@ -6001,7 +5995,7 @@
         <v>39971</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:4" s="6" customFormat="1">
@@ -6015,7 +6009,7 @@
         <v>39971</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="153" spans="1:4" s="6" customFormat="1">
@@ -6029,7 +6023,7 @@
         <v>39972</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="154" spans="1:4" s="6" customFormat="1">
@@ -6037,7 +6031,7 @@
         <v>54</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C154" s="7">
         <v>39972</v>
@@ -6071,7 +6065,7 @@
         <v>39972</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="157" spans="1:4" s="6" customFormat="1">
@@ -6084,65 +6078,55 @@
       <c r="C159" s="7"/>
     </row>
     <row r="160" spans="1:4" s="3" customFormat="1"/>
-    <row r="161" spans="2:4" s="3" customFormat="1"/>
-    <row r="162" spans="2:4" s="4" customFormat="1" ht="26.25">
+    <row r="161" spans="3:4" s="3" customFormat="1"/>
+    <row r="162" spans="3:4" s="4" customFormat="1" ht="26.25">
       <c r="D162" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="163" spans="2:4" s="3" customFormat="1"/>
-    <row r="164" spans="2:4" s="3" customFormat="1"/>
-    <row r="165" spans="2:4" s="4" customFormat="1" ht="26.25">
+    <row r="163" spans="3:4" s="3" customFormat="1"/>
+    <row r="164" spans="3:4" s="3" customFormat="1"/>
+    <row r="165" spans="3:4" s="4" customFormat="1" ht="26.25">
       <c r="D165" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="2:4" s="2" customFormat="1">
+    <row r="166" spans="3:4" s="2" customFormat="1">
       <c r="C166" s="15"/>
       <c r="D166" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="167" spans="2:4" s="2" customFormat="1">
-      <c r="B167" s="2" t="s">
-        <v>187</v>
-      </c>
+    <row r="167" spans="3:4" s="2" customFormat="1">
       <c r="D167" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="168" spans="2:4" s="2" customFormat="1">
-      <c r="B168" s="2" t="s">
-        <v>53</v>
-      </c>
+    <row r="168" spans="3:4" s="2" customFormat="1">
       <c r="D168" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4" s="2" customFormat="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="169" spans="3:4" s="2" customFormat="1">
       <c r="D169" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" s="2" customFormat="1">
-      <c r="D170" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" s="2" customFormat="1"/>
-    <row r="172" spans="2:4" s="3" customFormat="1"/>
-    <row r="173" spans="2:4" s="3" customFormat="1"/>
-    <row r="174" spans="2:4" s="4" customFormat="1" ht="26.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="3:4" s="2" customFormat="1"/>
+    <row r="171" spans="3:4" s="2" customFormat="1"/>
+    <row r="172" spans="3:4" s="3" customFormat="1"/>
+    <row r="173" spans="3:4" s="3" customFormat="1"/>
+    <row r="174" spans="3:4" s="4" customFormat="1" ht="26.25">
       <c r="D174" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="175" spans="2:4" s="10" customFormat="1">
+    <row r="175" spans="3:4" s="10" customFormat="1">
       <c r="D175" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="176" spans="2:4" s="3" customFormat="1"/>
+    <row r="176" spans="3:4" s="3" customFormat="1"/>
     <row r="177" spans="2:4" s="3" customFormat="1"/>
     <row r="178" spans="2:4" s="4" customFormat="1" ht="26.25">
       <c r="D178" s="5" t="s">
@@ -6421,10 +6405,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="C9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6490,13 +6474,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" t="s">
         <v>193</v>
-      </c>
-      <c r="F1" t="s">
-        <v>195</v>
       </c>
       <c r="H1">
         <v>585</v>
@@ -6508,13 +6492,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
         <v>192</v>
       </c>
-      <c r="C2" t="s">
-        <v>194</v>
-      </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H2">
         <v>717</v>

</xml_diff>